<commit_message>
API Automation 22nd Jan
</commit_message>
<xml_diff>
--- a/src/test/resources/data/BulkUpload_API_Valid.xlsx
+++ b/src/test/resources/data/BulkUpload_API_Valid.xlsx
@@ -19,7 +19,7 @@
     <sheet name="Rules" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Upload Template'!$A$1:$Q$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Upload Template'!$A$1:$Q$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1011,9 +1011,6 @@
     <t>Acrewood Nursery LTD</t>
   </si>
   <si>
-    <t>B13943</t>
-  </si>
-  <si>
     <t>SC229641</t>
   </si>
   <si>
@@ -1026,18 +1023,12 @@
     <t>SC270780</t>
   </si>
   <si>
-    <t>SB0407</t>
-  </si>
-  <si>
     <t>SC231967</t>
   </si>
   <si>
     <t>Micro Organisation</t>
   </si>
   <si>
-    <t>CR20503</t>
-  </si>
-  <si>
     <t>SC10000</t>
   </si>
   <si>
@@ -1330,6 +1321,15 @@
   </si>
   <si>
     <t>UKSA</t>
+  </si>
+  <si>
+    <t>CR205039</t>
+  </si>
+  <si>
+    <t>BC139439</t>
+  </si>
+  <si>
+    <t>SB040709</t>
   </si>
 </sst>
 </file>
@@ -1517,7 +1517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1635,9 +1635,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1972,9 +1969,9 @@
   <dimension ref="A1:Q1351"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z29" sqref="Z29"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20" x14ac:dyDescent="0.35"/>
@@ -2053,7 +2050,7 @@
     </row>
     <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B2" s="28" t="s">
         <v>187</v>
@@ -2102,10 +2099,10 @@
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="28" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C3" s="41" t="s">
         <v>66</v>
@@ -2155,7 +2152,7 @@
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="28" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B4" s="28" t="s">
         <v>188</v>
@@ -2204,10 +2201,10 @@
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="28" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C5" s="41" t="s">
         <v>44</v>
@@ -2253,7 +2250,7 @@
     </row>
     <row r="6" spans="1:17" s="1" customFormat="1" ht="80" x14ac:dyDescent="0.35">
       <c r="A6" s="28" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B6" s="28" t="s">
         <v>189</v>
@@ -2285,7 +2282,7 @@
         <v>196</v>
       </c>
       <c r="M6" s="38" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="N6" s="42">
         <v>43994</v>
@@ -2302,10 +2299,10 @@
     </row>
     <row r="7" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="28" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C7" s="41" t="s">
         <v>73</v>
@@ -2351,10 +2348,10 @@
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="28" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C8" s="41" t="s">
         <v>15</v>
@@ -2373,8 +2370,8 @@
       <c r="I8" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="43" t="s">
-        <v>233</v>
+      <c r="J8" s="34" t="s">
+        <v>329</v>
       </c>
       <c r="K8" s="29" t="s">
         <v>204</v>
@@ -2383,7 +2380,7 @@
         <v>205</v>
       </c>
       <c r="M8" s="38" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N8" s="42">
         <v>42982</v>
@@ -2400,10 +2397,10 @@
     </row>
     <row r="9" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="28" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C9" s="41" t="s">
         <v>15</v>
@@ -2432,7 +2429,7 @@
         <v>58</v>
       </c>
       <c r="M9" s="38" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="N9" s="42">
         <v>43327</v>
@@ -2449,10 +2446,10 @@
     </row>
     <row r="10" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="28" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C10" s="41" t="s">
         <v>75</v>
@@ -2471,8 +2468,8 @@
       <c r="I10" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="43" t="s">
-        <v>233</v>
+      <c r="J10" s="34" t="s">
+        <v>329</v>
       </c>
       <c r="K10" s="29" t="s">
         <v>204</v>
@@ -2498,10 +2495,10 @@
     </row>
     <row r="11" spans="1:17" s="1" customFormat="1" ht="40" x14ac:dyDescent="0.35">
       <c r="A11" s="28" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C11" s="41" t="s">
         <v>49</v>
@@ -2530,7 +2527,7 @@
         <v>200</v>
       </c>
       <c r="M11" s="38" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="N11" s="42">
         <v>43108</v>
@@ -2547,10 +2544,10 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="28" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C12" s="41" t="s">
         <v>72</v>
@@ -2569,8 +2566,8 @@
       <c r="I12" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="J12" s="43" t="s">
-        <v>233</v>
+      <c r="J12" s="34" t="s">
+        <v>329</v>
       </c>
       <c r="K12" s="29" t="s">
         <v>204</v>
@@ -2579,7 +2576,7 @@
         <v>14</v>
       </c>
       <c r="M12" s="38" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="N12" s="42">
         <v>43534</v>
@@ -2599,7 +2596,7 @@
         <v>194</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C13" s="41" t="s">
         <v>15</v>
@@ -2618,8 +2615,8 @@
       <c r="I13" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="J13" s="43" t="s">
-        <v>233</v>
+      <c r="J13" s="34" t="s">
+        <v>329</v>
       </c>
       <c r="K13" s="29" t="s">
         <v>204</v>
@@ -2628,7 +2625,7 @@
         <v>58</v>
       </c>
       <c r="M13" s="38" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="N13" s="42">
         <v>43593</v>
@@ -2645,10 +2642,10 @@
     </row>
     <row r="14" spans="1:17" ht="40" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C14" s="41" t="s">
         <v>15</v>
@@ -2677,7 +2674,7 @@
         <v>58</v>
       </c>
       <c r="M14" s="38" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="N14" s="42">
         <v>43992</v>
@@ -2694,10 +2691,10 @@
     </row>
     <row r="15" spans="1:17" ht="40" x14ac:dyDescent="0.35">
       <c r="A15" s="28" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C15" s="41" t="s">
         <v>46</v>
@@ -2726,7 +2723,7 @@
         <v>58</v>
       </c>
       <c r="M15" s="38" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="N15" s="42">
         <v>43167</v>
@@ -2746,7 +2743,7 @@
         <v>198</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C16" s="41" t="s">
         <v>15</v>
@@ -2765,8 +2762,8 @@
       <c r="I16" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="J16" s="43" t="s">
-        <v>233</v>
+      <c r="J16" s="34" t="s">
+        <v>329</v>
       </c>
       <c r="K16" s="29" t="s">
         <v>204</v>
@@ -2775,7 +2772,7 @@
         <v>14</v>
       </c>
       <c r="M16" s="38" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="N16" s="42">
         <v>42584</v>
@@ -2792,10 +2789,10 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="28" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C17" s="41" t="s">
         <v>72</v>
@@ -2824,7 +2821,7 @@
         <v>58</v>
       </c>
       <c r="M17" s="38" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="N17" s="42">
         <v>42686</v>
@@ -2844,7 +2841,7 @@
         <v>202</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C18" s="41" t="s">
         <v>73</v>
@@ -2863,8 +2860,8 @@
       <c r="I18" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="J18" s="43" t="s">
-        <v>233</v>
+      <c r="J18" s="34" t="s">
+        <v>329</v>
       </c>
       <c r="K18" s="29" t="s">
         <v>204</v>
@@ -2873,7 +2870,7 @@
         <v>14</v>
       </c>
       <c r="M18" s="38" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="N18" s="42">
         <v>44117</v>
@@ -2890,10 +2887,10 @@
     </row>
     <row r="19" spans="1:17" ht="40" x14ac:dyDescent="0.35">
       <c r="A19" s="28" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C19" s="41" t="s">
         <v>73</v>
@@ -2922,7 +2919,7 @@
         <v>55</v>
       </c>
       <c r="M19" s="38" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="N19" s="42">
         <v>44104</v>
@@ -2939,10 +2936,10 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="28" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C20" s="41" t="s">
         <v>73</v>
@@ -2962,16 +2959,16 @@
         <v>8</v>
       </c>
       <c r="J20" s="34" t="s">
-        <v>225</v>
+        <v>330</v>
       </c>
       <c r="K20" s="29" t="s">
         <v>218</v>
       </c>
       <c r="L20" s="38" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="M20" s="38" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="N20" s="42">
         <v>44105</v>
@@ -3009,13 +3006,13 @@
         <v>8</v>
       </c>
       <c r="J21" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K21" s="29" t="s">
         <v>219</v>
       </c>
       <c r="L21" s="38" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="M21" s="38" t="s">
         <v>208</v>
@@ -3038,7 +3035,7 @@
         <v>207</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C22" s="41" t="s">
         <v>73</v>
@@ -3058,7 +3055,7 @@
         <v>8</v>
       </c>
       <c r="J22" s="34" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K22" s="29" t="s">
         <v>220</v>
@@ -3067,7 +3064,7 @@
         <v>200</v>
       </c>
       <c r="M22" s="38" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="N22" s="42">
         <v>44105</v>
@@ -3084,10 +3081,10 @@
     </row>
     <row r="23" spans="1:17" ht="60" x14ac:dyDescent="0.35">
       <c r="A23" s="28" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C23" s="41" t="s">
         <v>73</v>
@@ -3107,7 +3104,7 @@
         <v>8</v>
       </c>
       <c r="J23" s="34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K23" s="29" t="s">
         <v>221</v>
@@ -3136,7 +3133,7 @@
         <v>210</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C24" s="41" t="s">
         <v>73</v>
@@ -3156,16 +3153,16 @@
         <v>8</v>
       </c>
       <c r="J24" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K24" s="29" t="s">
         <v>222</v>
       </c>
       <c r="L24" s="38" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="M24" s="38" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="N24" s="42">
         <v>44105</v>
@@ -3182,10 +3179,10 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="28" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C25" s="41" t="s">
         <v>73</v>
@@ -3205,16 +3202,16 @@
         <v>8</v>
       </c>
       <c r="J25" s="34" t="s">
-        <v>230</v>
+        <v>331</v>
       </c>
       <c r="K25" s="29" t="s">
         <v>223</v>
       </c>
       <c r="L25" s="38" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="M25" s="38" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="N25" s="42">
         <v>44105</v>
@@ -3231,10 +3228,10 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="28" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C26" s="41" t="s">
         <v>73</v>
@@ -3254,7 +3251,7 @@
         <v>8</v>
       </c>
       <c r="J26" s="34" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K26" s="29" t="s">
         <v>224</v>
@@ -3263,7 +3260,7 @@
         <v>196</v>
       </c>
       <c r="M26" s="38" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="N26" s="42">
         <v>44105</v>
@@ -15068,6 +15065,7 @@
       <c r="D1351" s="22"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Q1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -15144,7 +15142,7 @@
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C1" t="s">
         <v>187</v>
@@ -15158,10 +15156,10 @@
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -15172,7 +15170,7 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C3" t="s">
         <v>188</v>
@@ -15186,10 +15184,10 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C4" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -15200,7 +15198,7 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C5" t="s">
         <v>189</v>
@@ -15209,15 +15207,15 @@
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C6" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E6">
         <v>6</v>
@@ -15228,38 +15226,38 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E7">
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C8" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E8">
         <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C9" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E9">
         <v>9</v>
@@ -15270,30 +15268,30 @@
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C10" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E10">
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C11" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E11">
         <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
@@ -15301,41 +15299,41 @@
         <v>194</v>
       </c>
       <c r="C12" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E12">
         <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C13" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E13">
         <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C14" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E14">
         <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.35">
@@ -15343,27 +15341,27 @@
         <v>198</v>
       </c>
       <c r="C15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E15">
         <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C16" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E16">
         <v>16</v>
       </c>
       <c r="F16" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.35">
@@ -15371,41 +15369,41 @@
         <v>202</v>
       </c>
       <c r="C17" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E17">
         <v>17</v>
       </c>
       <c r="F17" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C18" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E18">
         <v>18</v>
       </c>
       <c r="F18" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C19" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E19">
         <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.35">
@@ -15413,7 +15411,7 @@
         <v>206</v>
       </c>
       <c r="C20" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E20">
         <v>20</v>
@@ -15427,21 +15425,21 @@
         <v>207</v>
       </c>
       <c r="C21" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E21">
         <v>21</v>
       </c>
       <c r="F21" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C22" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E22">
         <v>22</v>
@@ -15455,41 +15453,41 @@
         <v>210</v>
       </c>
       <c r="C23" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E23">
         <v>23</v>
       </c>
       <c r="F23" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C24" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E24">
         <v>24</v>
       </c>
       <c r="F24" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C25" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E25">
         <v>25</v>
       </c>
       <c r="F25" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.35">
@@ -15497,7 +15495,7 @@
         <v>26</v>
       </c>
       <c r="F26" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.35">
@@ -15505,7 +15503,7 @@
         <v>27</v>
       </c>
       <c r="F27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.35">
@@ -15513,7 +15511,7 @@
         <v>28</v>
       </c>
       <c r="F28" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.35">
@@ -15521,7 +15519,7 @@
         <v>29</v>
       </c>
       <c r="F29" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.35">
@@ -15529,7 +15527,7 @@
         <v>30</v>
       </c>
       <c r="F30" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.35">
@@ -15537,7 +15535,7 @@
         <v>31</v>
       </c>
       <c r="F31" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.35">
@@ -15545,7 +15543,7 @@
         <v>32</v>
       </c>
       <c r="F32" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="33" spans="5:6" x14ac:dyDescent="0.35">
@@ -15553,7 +15551,7 @@
         <v>33</v>
       </c>
       <c r="F33" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="34" spans="5:6" x14ac:dyDescent="0.35">
@@ -15561,7 +15559,7 @@
         <v>34</v>
       </c>
       <c r="F34" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="35" spans="5:6" x14ac:dyDescent="0.35">
@@ -15569,7 +15567,7 @@
         <v>35</v>
       </c>
       <c r="F35" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="36" spans="5:6" x14ac:dyDescent="0.35">
@@ -15577,7 +15575,7 @@
         <v>36</v>
       </c>
       <c r="F36" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="37" spans="5:6" x14ac:dyDescent="0.35">
@@ -15585,7 +15583,7 @@
         <v>37</v>
       </c>
       <c r="F37" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="38" spans="5:6" x14ac:dyDescent="0.35">
@@ -15593,7 +15591,7 @@
         <v>38</v>
       </c>
       <c r="F38" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="39" spans="5:6" x14ac:dyDescent="0.35">
@@ -15601,7 +15599,7 @@
         <v>39</v>
       </c>
       <c r="F39" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="40" spans="5:6" x14ac:dyDescent="0.35">
@@ -15609,7 +15607,7 @@
         <v>40</v>
       </c>
       <c r="F40" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="41" spans="5:6" x14ac:dyDescent="0.35">
@@ -15617,7 +15615,7 @@
         <v>41</v>
       </c>
       <c r="F41" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="42" spans="5:6" x14ac:dyDescent="0.35">
@@ -15625,7 +15623,7 @@
         <v>42</v>
       </c>
       <c r="F42" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="43" spans="5:6" x14ac:dyDescent="0.35">
@@ -15633,7 +15631,7 @@
         <v>43</v>
       </c>
       <c r="F43" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="44" spans="5:6" x14ac:dyDescent="0.35">
@@ -15641,7 +15639,7 @@
         <v>44</v>
       </c>
       <c r="F44" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="45" spans="5:6" x14ac:dyDescent="0.35">
@@ -15649,7 +15647,7 @@
         <v>45</v>
       </c>
       <c r="F45" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="46" spans="5:6" x14ac:dyDescent="0.35">
@@ -15657,7 +15655,7 @@
         <v>46</v>
       </c>
       <c r="F46" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="47" spans="5:6" x14ac:dyDescent="0.35">
@@ -15665,7 +15663,7 @@
         <v>47</v>
       </c>
       <c r="F47" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="48" spans="5:6" x14ac:dyDescent="0.35">
@@ -15681,7 +15679,7 @@
         <v>49</v>
       </c>
       <c r="F49" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="50" spans="5:6" x14ac:dyDescent="0.35">
@@ -15689,7 +15687,7 @@
         <v>50</v>
       </c>
       <c r="F50" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="51" spans="5:6" x14ac:dyDescent="0.35">
@@ -15697,7 +15695,7 @@
         <v>51</v>
       </c>
       <c r="F51" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="52" spans="5:6" x14ac:dyDescent="0.35">
@@ -15705,7 +15703,7 @@
         <v>52</v>
       </c>
       <c r="F52" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="53" spans="5:6" x14ac:dyDescent="0.35">
@@ -15713,7 +15711,7 @@
         <v>53</v>
       </c>
       <c r="F53" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="54" spans="5:6" x14ac:dyDescent="0.35">
@@ -15721,7 +15719,7 @@
         <v>54</v>
       </c>
       <c r="F54" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="55" spans="5:6" x14ac:dyDescent="0.35">
@@ -15729,7 +15727,7 @@
         <v>55</v>
       </c>
       <c r="F55" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="56" spans="5:6" x14ac:dyDescent="0.35">
@@ -15737,7 +15735,7 @@
         <v>56</v>
       </c>
       <c r="F56" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="57" spans="5:6" x14ac:dyDescent="0.35">
@@ -15745,7 +15743,7 @@
         <v>57</v>
       </c>
       <c r="F57" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="58" spans="5:6" x14ac:dyDescent="0.35">
@@ -15753,7 +15751,7 @@
         <v>58</v>
       </c>
       <c r="F58" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="59" spans="5:6" x14ac:dyDescent="0.35">
@@ -15769,7 +15767,7 @@
         <v>60</v>
       </c>
       <c r="F60" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="61" spans="5:6" x14ac:dyDescent="0.35">
@@ -15777,7 +15775,7 @@
         <v>61</v>
       </c>
       <c r="F61" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="62" spans="5:6" x14ac:dyDescent="0.35">
@@ -15785,7 +15783,7 @@
         <v>62</v>
       </c>
       <c r="F62" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="63" spans="5:6" x14ac:dyDescent="0.35">
@@ -15793,7 +15791,7 @@
         <v>63</v>
       </c>
       <c r="F63" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="64" spans="5:6" x14ac:dyDescent="0.35">
@@ -15801,7 +15799,7 @@
         <v>64</v>
       </c>
       <c r="F64" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="65" spans="5:6" x14ac:dyDescent="0.35">
@@ -15809,7 +15807,7 @@
         <v>65</v>
       </c>
       <c r="F65" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="66" spans="5:6" x14ac:dyDescent="0.35">
@@ -15817,7 +15815,7 @@
         <v>66</v>
       </c>
       <c r="F66" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="67" spans="5:6" x14ac:dyDescent="0.35">
@@ -15825,7 +15823,7 @@
         <v>67</v>
       </c>
       <c r="F67" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -16600,13 +16598,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="46" t="s">
         <v>162</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="46" t="s">
         <v>152</v>
       </c>
       <c r="D2" s="29" t="s">
@@ -16614,37 +16612,37 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="48"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
+      <c r="A3" s="47"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
       <c r="D3" s="29" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
       <c r="D4" s="29" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="49"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
       <c r="D5" s="29" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="43" t="s">
         <v>148</v>
       </c>
       <c r="D6" s="15" t="s">
@@ -16652,25 +16650,25 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="45"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
+      <c r="A7" s="44"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="15" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="45"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
+      <c r="A8" s="44"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="29" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="46"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
+      <c r="A9" s="45"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
       <c r="D9" s="29" t="s">
         <v>169</v>
       </c>
@@ -16767,13 +16765,13 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="43" t="s">
         <v>165</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="43" t="s">
         <v>113</v>
       </c>
       <c r="D17" s="33" t="s">
@@ -16781,33 +16779,33 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="45"/>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
       <c r="D18" s="33" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="45"/>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
       <c r="D19" s="33" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="45"/>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45"/>
+      <c r="A20" s="44"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
       <c r="D20" s="33" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="46"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="46"/>
+      <c r="A21" s="45"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
       <c r="D21" s="29" t="s">
         <v>169</v>
       </c>
@@ -16974,65 +16972,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095552673811A1544B9DC17E80367E3D9" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f9926b2f923abdc963915abbe4b5426c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ff8cd83-fc61-4182-af0d-9444b096b4cc" xmlns:ns3="0063f72e-ace3-48fb-9c1f-5b513408b31f" xmlns:ns4="b413c3fd-5a3b-4239-b985-69032e371c04" xmlns:ns5="a8f60570-4bd3-4f2b-950b-a996de8ab151" xmlns:ns6="aaacb922-5235-4a66-b188-303b9b46fbd7" xmlns:ns7="58eecf05-07e6-460c-a17a-1e6913e0d7ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ce3640aaef15d750e87a37a534cff0e6" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="" ns7:_="">
     <xsd:import namespace="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
@@ -17386,7 +17325,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
@@ -17421,23 +17360,66 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{501657FE-465F-48E5-871D-013E453FC850}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17460,7 +17442,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
@@ -17479,4 +17461,20 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>